<commit_message>
29th July 2022 - Session
</commit_message>
<xml_diff>
--- a/Online Exam DB Plan.xlsx
+++ b/Online Exam DB Plan.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af790a540ce3e87d/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ns_neutron\neutron_sql_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A6E6145-4BDC-49CC-8A75-A28697423426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAAA9B8-2B46-4FD2-B4F3-DD3FAF76E2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>Types of login - candidate &lt; teachers &lt; admin</t>
   </si>
@@ -154,15 +155,6 @@
     <t>course</t>
   </si>
   <si>
-    <t>graduatioyear</t>
-  </si>
-  <si>
-    <t>account creation date</t>
-  </si>
-  <si>
-    <t>last active date</t>
-  </si>
-  <si>
     <t>usertype</t>
   </si>
   <si>
@@ -230,13 +222,52 @@
   </si>
   <si>
     <t>submission</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
+    <t>%@gmail.com</t>
+  </si>
+  <si>
+    <t>test@gmail.com123</t>
+  </si>
+  <si>
+    <t>deepak@gmail.com</t>
+  </si>
+  <si>
+    <t>deepak@test.com</t>
+  </si>
+  <si>
+    <t>deepak%</t>
+  </si>
+  <si>
+    <t>%yahoo%</t>
+  </si>
+  <si>
+    <t>WHERE</t>
+  </si>
+  <si>
+    <t>LIKE</t>
+  </si>
+  <si>
+    <t>gradyear</t>
+  </si>
+  <si>
+    <t>accountdate</t>
+  </si>
+  <si>
+    <t>lastdate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +279,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,14 +309,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,7 +635,7 @@
   <dimension ref="B3:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,33 +658,33 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M4" t="s">
         <v>20</v>
@@ -656,10 +698,10 @@
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
@@ -673,7 +715,7 @@
         <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
@@ -687,7 +729,7 @@
         <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
@@ -698,7 +740,7 @@
         <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
@@ -712,7 +754,7 @@
         <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
@@ -723,7 +765,7 @@
         <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
@@ -731,13 +773,13 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G11" t="s">
         <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
@@ -748,7 +790,7 @@
         <v>35</v>
       </c>
       <c r="I12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
@@ -756,7 +798,7 @@
         <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
@@ -764,7 +806,7 @@
         <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
@@ -775,7 +817,7 @@
         <v>38</v>
       </c>
       <c r="I15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
@@ -783,12 +825,12 @@
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G17" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -796,7 +838,7 @@
         <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -841,27 +883,27 @@
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
@@ -888,4 +930,71 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D047279D-6843-4792-A616-C081EA17B349}">
+  <dimension ref="A3:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D11" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{2DB421F9-79E4-4F55-A502-14D8ABDB7EEA}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{43795DA6-0503-4E96-85CD-473AC32BB92A}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{14B10A45-F8C4-4D30-9597-67407D773663}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{6F77E28D-A89C-4DA6-88F6-D7D9B66875B4}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{66DF47D0-599D-44D4-89AB-3BB4F43049BC}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{FB329F14-8908-4329-8EF6-3FFFB85554A0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1st August 2022 - Session
</commit_message>
<xml_diff>
--- a/Online Exam DB Plan.xlsx
+++ b/Online Exam DB Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ns_neutron\neutron_sql_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAAA9B8-2B46-4FD2-B4F3-DD3FAF76E2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9C20B4-B945-4B38-8721-714220E0B82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
   </bookViews>
@@ -292,12 +292,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -313,10 +319,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -635,7 +642,7 @@
   <dimension ref="B3:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +701,7 @@
       <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
@@ -708,7 +715,7 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">

</xml_diff>

<commit_message>
4th August 2022 - Session
</commit_message>
<xml_diff>
--- a/Online Exam DB Plan.xlsx
+++ b/Online Exam DB Plan.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ns_neutron\neutron_sql_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9C20B4-B945-4B38-8721-714220E0B82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A00B381-745E-45B4-8E29-CAD5594D250F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="API" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="169">
   <si>
     <t>Types of login - candidate &lt; teachers &lt; admin</t>
   </si>
@@ -261,13 +263,295 @@
   </si>
   <si>
     <t>lastdate</t>
+  </si>
+  <si>
+    <t>LOGIN</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Create an account</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/users/adduser</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/users/login</t>
+  </si>
+  <si>
+    <t>Update User Details</t>
+  </si>
+  <si>
+    <t>All Users list</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/users/allusers</t>
+  </si>
+  <si>
+    <t>Single User Search</t>
+  </si>
+  <si>
+    <t>Return all fields</t>
+  </si>
+  <si>
+    <t>Return all fields but not password</t>
+  </si>
+  <si>
+    <t>GET/POST</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/users/removeuser</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/users/updateuser</t>
+  </si>
+  <si>
+    <t>Types of keys</t>
+  </si>
+  <si>
+    <t>Foreign</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Super</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>Candidate</t>
+  </si>
+  <si>
+    <t>Alternate</t>
+  </si>
+  <si>
+    <t>Composite</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>order details</t>
+  </si>
+  <si>
+    <t>orderid</t>
+  </si>
+  <si>
+    <t>foodid</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>roti</t>
+  </si>
+  <si>
+    <t>paneer</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>salad</t>
+  </si>
+  <si>
+    <t>dal</t>
+  </si>
+  <si>
+    <t>connects with primary key of another table</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>can be multiple</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>null is possible</t>
+  </si>
+  <si>
+    <t>duplicate possible</t>
+  </si>
+  <si>
+    <t>pupilicate not possible</t>
+  </si>
+  <si>
+    <t>auto increment possible</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>value modification not possible</t>
+  </si>
+  <si>
+    <t>value modification possible</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>studentid</t>
+  </si>
+  <si>
+    <t>Student Course</t>
+  </si>
+  <si>
+    <t>courseid</t>
+  </si>
+  <si>
+    <t>coursename</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>lmn</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>sdfaef</t>
+  </si>
+  <si>
+    <t>efawef</t>
+  </si>
+  <si>
+    <t>WFEWEF</t>
+  </si>
+  <si>
+    <t>WEFwfe</t>
+  </si>
+  <si>
+    <t>java</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>js</t>
+  </si>
+  <si>
+    <t>cloud</t>
+  </si>
+  <si>
+    <t>php</t>
+  </si>
+  <si>
+    <t>dot net</t>
+  </si>
+  <si>
+    <t>dbms</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>1 - java</t>
+  </si>
+  <si>
+    <t>2 - python</t>
+  </si>
+  <si>
+    <t>3 - js</t>
+  </si>
+  <si>
+    <t>4 - cloud</t>
+  </si>
+  <si>
+    <t>7 - dbms</t>
+  </si>
+  <si>
+    <t>fsff</t>
+  </si>
+  <si>
+    <t>sdsf</t>
+  </si>
+  <si>
+    <t>cross join</t>
+  </si>
+  <si>
+    <t>self join</t>
+  </si>
+  <si>
+    <t>inner</t>
+  </si>
+  <si>
+    <t>outer</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>union</t>
+  </si>
+  <si>
+    <t>intersection</t>
+  </si>
+  <si>
+    <t>inner join</t>
+  </si>
+  <si>
+    <t>all students with course name</t>
+  </si>
+  <si>
+    <t>all student names who are enrolled in any course</t>
+  </si>
+  <si>
+    <t>left join</t>
+  </si>
+  <si>
+    <t>right join</t>
+  </si>
+  <si>
+    <t>all courses with student names</t>
+  </si>
+  <si>
+    <t>full join/ outer join</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/users/searchuser/id005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,8 +575,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,7 +607,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,11 +655,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -641,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598E409D-B184-44C1-9772-DD09FE403E30}">
   <dimension ref="B3:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,10 +1058,10 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I4" t="s">
@@ -698,10 +1072,10 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="6" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
@@ -715,7 +1089,7 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G6" t="s">
@@ -729,7 +1103,7 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G7" t="s">
@@ -765,7 +1139,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
+      <c r="F10" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G10" t="s">
@@ -801,6 +1175,9 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="G13" t="s">
         <v>36</v>
       </c>
@@ -809,6 +1186,9 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="G14" t="s">
         <v>37</v>
       </c>
@@ -835,12 +1215,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="G17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -848,37 +1228,129 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>1111</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24">
+        <v>1111</v>
+      </c>
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>111</v>
+      </c>
+      <c r="F25" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25">
+        <v>1111</v>
+      </c>
+      <c r="H25" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>500</v>
+      </c>
+      <c r="F26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26">
+        <v>1111</v>
+      </c>
+      <c r="H26" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>1111</v>
+      </c>
+      <c r="H27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>1111</v>
+      </c>
+      <c r="H28" t="s">
+        <v>114</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>13</v>
       </c>
@@ -1004,4 +1476,1407 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71A6B84-5801-4404-B126-D1C859154014}">
+  <dimension ref="B3:O72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="12"/>
+    <col min="2" max="2" width="29.88671875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="15" style="12" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="12" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" style="12" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" style="12" customWidth="1"/>
+    <col min="8" max="10" width="8.88671875" style="12"/>
+    <col min="11" max="11" width="21" style="12" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" style="12" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" style="12" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="D6" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="D7" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="D8" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F13" s="16"/>
+      <c r="J13" s="16"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="J15" s="17"/>
+      <c r="K15" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B16" s="12">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="12">
+        <v>1212</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="J16" s="17"/>
+      <c r="K16" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="L16" s="12">
+        <v>2</v>
+      </c>
+      <c r="N16" s="12">
+        <v>1</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="12">
+        <v>2</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" s="12">
+        <v>123132</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="12">
+        <v>1</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="I17" s="12">
+        <v>2</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="L17" s="12">
+        <v>3</v>
+      </c>
+      <c r="N17" s="12">
+        <v>2</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B18" s="12">
+        <v>3</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="12">
+        <v>123123</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="12">
+        <v>2</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I18" s="12">
+        <v>1</v>
+      </c>
+      <c r="J18" s="17"/>
+      <c r="K18" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="L18" s="12">
+        <v>1</v>
+      </c>
+      <c r="N18" s="12">
+        <v>3</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B19" s="12">
+        <v>4</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="12">
+        <v>12313</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="12">
+        <v>3</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" s="12">
+        <v>3</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="L19" s="12">
+        <v>2</v>
+      </c>
+      <c r="N19" s="12">
+        <v>4</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="12">
+        <v>5</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="12">
+        <v>323</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="12">
+        <v>4</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="12">
+        <v>4</v>
+      </c>
+      <c r="J20" s="17"/>
+      <c r="K20" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="L20" s="12">
+        <v>1</v>
+      </c>
+      <c r="N20" s="12">
+        <v>5</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F21" s="17"/>
+      <c r="G21" s="12">
+        <v>5</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J21" s="17"/>
+      <c r="K21" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="L21" s="12">
+        <v>2</v>
+      </c>
+      <c r="N21" s="12">
+        <v>6</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F22" s="17"/>
+      <c r="G22" s="12">
+        <v>6</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="J22" s="17"/>
+      <c r="K22" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="L22" s="12">
+        <v>3</v>
+      </c>
+      <c r="N22" s="12">
+        <v>7</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F23" s="17"/>
+      <c r="G23" s="12">
+        <v>7</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="L23" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="L24" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="L25" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="L26" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F27" s="17"/>
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F28" s="17"/>
+      <c r="J28" s="17"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="F29" s="17"/>
+      <c r="J29" s="17"/>
+    </row>
+    <row r="30" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B31" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B32" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C33" s="12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C38" s="19">
+        <v>1</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="19">
+        <v>1212</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" s="18">
+        <v>1</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I38" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C39" s="20">
+        <v>2</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39" s="20">
+        <v>123132</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="G39" s="21">
+        <v>1</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="I39" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="19">
+        <v>3</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="19">
+        <v>123123</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G40" s="18">
+        <v>1</v>
+      </c>
+      <c r="H40" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I40" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C41" s="19">
+        <v>4</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" s="19">
+        <v>12313</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G41" s="18">
+        <v>1</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I41" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C42" s="19">
+        <v>5</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="19">
+        <v>323</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="18">
+        <v>1</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="I42" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="20">
+        <v>1</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E43" s="20">
+        <v>1212</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43" s="21">
+        <v>2</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="19">
+        <v>2</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E44" s="19">
+        <v>123132</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G44" s="18">
+        <v>2</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I44" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C45" s="19">
+        <v>3</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E45" s="19">
+        <v>123123</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G45" s="18">
+        <v>2</v>
+      </c>
+      <c r="H45" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I45" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C46" s="19">
+        <v>4</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E46" s="19">
+        <v>12313</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G46" s="18">
+        <v>2</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C47" s="19">
+        <v>5</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="19">
+        <v>323</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G47" s="18">
+        <v>2</v>
+      </c>
+      <c r="H47" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="I47" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C48" s="19">
+        <v>1</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E48" s="19">
+        <v>1212</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G48" s="18">
+        <v>3</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I48" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C49" s="19">
+        <v>2</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E49" s="19">
+        <v>123132</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G49" s="18">
+        <v>3</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I49" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C50" s="20">
+        <v>3</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" s="20">
+        <v>123123</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G50" s="21">
+        <v>3</v>
+      </c>
+      <c r="H50" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="I50" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C51" s="19">
+        <v>4</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51" s="19">
+        <v>12313</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G51" s="18">
+        <v>3</v>
+      </c>
+      <c r="H51" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I51" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C52" s="19">
+        <v>5</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E52" s="19">
+        <v>323</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G52" s="18">
+        <v>3</v>
+      </c>
+      <c r="H52" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I52" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C53" s="19">
+        <v>1</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E53" s="19">
+        <v>1212</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G53" s="18">
+        <v>4</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I53" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C54" s="19">
+        <v>2</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E54" s="19">
+        <v>123132</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G54" s="18">
+        <v>4</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I54" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C55" s="19">
+        <v>3</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E55" s="19">
+        <v>123123</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G55" s="18">
+        <v>4</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I55" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C56" s="20">
+        <v>4</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E56" s="20">
+        <v>12313</v>
+      </c>
+      <c r="F56" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="G56" s="21">
+        <v>4</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="I56" s="21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C57" s="19">
+        <v>5</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E57" s="19">
+        <v>323</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G57" s="18">
+        <v>4</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I57" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C58" s="19">
+        <v>1</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E58" s="19">
+        <v>1212</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G58" s="18">
+        <v>5</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I58" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C59" s="19">
+        <v>2</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" s="19">
+        <v>123132</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G59" s="18">
+        <v>5</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I59" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C60" s="19">
+        <v>3</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E60" s="19">
+        <v>123123</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G60" s="18">
+        <v>5</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I60" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C61" s="19">
+        <v>4</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E61" s="19">
+        <v>12313</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G61" s="18">
+        <v>5</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I61" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C62" s="19">
+        <v>5</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E62" s="19">
+        <v>323</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G62" s="18">
+        <v>5</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I62" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C63" s="19">
+        <v>1</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E63" s="19">
+        <v>1212</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G63" s="18">
+        <v>6</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I63" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C64" s="19">
+        <v>2</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E64" s="19">
+        <v>123132</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G64" s="18">
+        <v>6</v>
+      </c>
+      <c r="H64" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I64" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C65" s="19">
+        <v>3</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E65" s="19">
+        <v>123123</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G65" s="18">
+        <v>6</v>
+      </c>
+      <c r="H65" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I65" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C66" s="19">
+        <v>4</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E66" s="19">
+        <v>12313</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G66" s="18">
+        <v>6</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I66" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C67" s="19">
+        <v>5</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E67" s="19">
+        <v>323</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G67" s="18">
+        <v>6</v>
+      </c>
+      <c r="H67" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I67" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C68" s="19">
+        <v>1</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E68" s="19">
+        <v>1212</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="G68" s="18">
+        <v>7</v>
+      </c>
+      <c r="H68" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I68" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C69" s="19">
+        <v>2</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E69" s="19">
+        <v>123132</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="G69" s="18">
+        <v>7</v>
+      </c>
+      <c r="H69" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I69" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C70" s="19">
+        <v>3</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E70" s="19">
+        <v>123123</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="G70" s="18">
+        <v>7</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I70" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C71" s="19">
+        <v>4</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E71" s="19">
+        <v>12313</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="G71" s="18">
+        <v>7</v>
+      </c>
+      <c r="H71" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I71" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C72" s="19">
+        <v>5</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E72" s="19">
+        <v>323</v>
+      </c>
+      <c r="F72" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G72" s="18">
+        <v>7</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I72" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBCD982-A1F7-4F12-9554-A4111D34D39C}">
+  <dimension ref="A3:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="37" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{CF5B090D-923E-4F39-A190-24B68A4A347A}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{5FE462A3-D5BF-4639-9BF6-C95D99F65B44}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{D0EBD89A-D66D-4DE7-86DF-5DFE6CF72550}"/>
+    <hyperlink ref="F8" r:id="rId4" xr:uid="{18C25863-A0B6-42AA-9649-2C7EF3D9B6E3}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{3B0BBC9D-C2D9-4372-8F28-57C51CE84779}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
8th August 2022 - Session
</commit_message>
<xml_diff>
--- a/Online Exam DB Plan.xlsx
+++ b/Online Exam DB Plan.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ns_neutron\neutron_sql_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A00B381-745E-45B4-8E29-CAD5594D250F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9863D66D-0DB8-492F-981E-8A86A740334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="API" sheetId="3" r:id="rId4"/>
+    <sheet name="DB Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Features" sheetId="5" r:id="rId2"/>
+    <sheet name="misc" sheetId="2" r:id="rId3"/>
+    <sheet name="class - joins, keys" sheetId="4" r:id="rId4"/>
+    <sheet name="API" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="203">
   <si>
     <t>Types of login - candidate &lt; teachers &lt; admin</t>
   </si>
@@ -313,9 +314,6 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>http://localhost:4000/users/removeuser</t>
-  </si>
-  <si>
     <t>http://localhost:4000/users/updateuser</t>
   </si>
   <si>
@@ -334,9 +332,6 @@
     <t>Super</t>
   </si>
   <si>
-    <t>dob</t>
-  </si>
-  <si>
     <t>Candidate</t>
   </si>
   <si>
@@ -346,45 +341,12 @@
     <t>Composite</t>
   </si>
   <si>
-    <t>orders</t>
-  </si>
-  <si>
-    <t>order details</t>
-  </si>
-  <si>
-    <t>orderid</t>
-  </si>
-  <si>
-    <t>foodid</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
     <t>phone</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
     <t>abc</t>
   </si>
   <si>
-    <t>roti</t>
-  </si>
-  <si>
-    <t>paneer</t>
-  </si>
-  <si>
-    <t>rice</t>
-  </si>
-  <si>
-    <t>salad</t>
-  </si>
-  <si>
-    <t>dal</t>
-  </si>
-  <si>
     <t>connects with primary key of another table</t>
   </si>
   <si>
@@ -545,6 +507,147 @@
   </si>
   <si>
     <t>http://localhost:4000/users/searchuser/id005</t>
+  </si>
+  <si>
+    <t>subject_id</t>
+  </si>
+  <si>
+    <t>subject_name</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+  </si>
+  <si>
+    <t>EXAMLOG</t>
+  </si>
+  <si>
+    <t>EXAMLOG_DETAILS</t>
+  </si>
+  <si>
+    <t>teacher_id</t>
+  </si>
+  <si>
+    <t>default value 4</t>
+  </si>
+  <si>
+    <t>default value 1</t>
+  </si>
+  <si>
+    <t>optional/int - default value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample </t>
+  </si>
+  <si>
+    <t>https://dev-quiz-react.vercel.app/login</t>
+  </si>
+  <si>
+    <t>testbook</t>
+  </si>
+  <si>
+    <t>varchar(500) - NOT NULL</t>
+  </si>
+  <si>
+    <t>varchar(20) - NOT NULL</t>
+  </si>
+  <si>
+    <t>varchar(200) - NOT NULL</t>
+  </si>
+  <si>
+    <t>int() - 1/2/3/4/5 - NOT NULL</t>
+  </si>
+  <si>
+    <t>math - 1</t>
+  </si>
+  <si>
+    <t>gk - 2</t>
+  </si>
+  <si>
+    <t>history - 3</t>
+  </si>
+  <si>
+    <t>computer - 4</t>
+  </si>
+  <si>
+    <t>programming - 5</t>
+  </si>
+  <si>
+    <t>english - 6</t>
+  </si>
+  <si>
+    <t>aptitude - 7</t>
+  </si>
+  <si>
+    <t>questions</t>
+  </si>
+  <si>
+    <t>ADD question</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/questions/addquestion</t>
+  </si>
+  <si>
+    <t>DELETE QS</t>
+  </si>
+  <si>
+    <t>EDIT QS</t>
+  </si>
+  <si>
+    <t>GET ALL QS</t>
+  </si>
+  <si>
+    <t>GET ALL BY SUBJECT ID</t>
+  </si>
+  <si>
+    <t>GET ONE SPECIFIC QS</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/questions/editquestion</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Body - subject_id,question,answer1,answer2,answer3,answer4,correctanswer</t>
+  </si>
+  <si>
+    <t>Body - qs_id, subject_id,question,answer1,answer2,answer3,answer4,correctanswer</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/questions/removequestion/qs_id</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/questions/searchquestion/qs_id</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/questions/getquestions</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/questions/getquestionbysubject/subject_id</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/users/removeuser/userid</t>
+  </si>
+  <si>
+    <t>body - userid</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>userid and password</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>TYPE</t>
   </si>
 </sst>
 </file>
@@ -598,7 +701,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -641,6 +744,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -655,7 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -698,6 +807,8 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1013,397 +1124,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598E409D-B184-44C1-9772-DD09FE403E30}">
-  <dimension ref="B3:P47"/>
+  <dimension ref="C3:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="9" max="11" width="13" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
+    <col min="2" max="2" width="3.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" style="23" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="8" max="8" width="3.109375" style="23" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+    <col min="10" max="10" width="3.109375" style="23" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="3.109375" style="23" customWidth="1"/>
+    <col min="14" max="14" width="18.5546875" customWidth="1"/>
+    <col min="15" max="15" width="3.109375" style="23" customWidth="1"/>
+    <col min="16" max="16" width="14.77734375" customWidth="1"/>
+    <col min="17" max="17" width="17.21875" customWidth="1"/>
+    <col min="18" max="18" width="3.109375" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
+    <row r="3" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="22"/>
       <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="J3" s="22"/>
       <c r="K3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="L3" s="22"/>
       <c r="M3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="22"/>
       <c r="P3" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F4" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="R3" s="22"/>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
+      <c r="F4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M4" t="s">
+      <c r="G4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G5" t="s">
+        <v>170</v>
+      </c>
+      <c r="I5" t="s">
+        <v>157</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
+    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>169</v>
+      </c>
+      <c r="K6" t="s">
         <v>41</v>
       </c>
-      <c r="M5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
+    </row>
+    <row r="7" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
       <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>3</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F10" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C10" s="11" t="s">
         <v>32</v>
       </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
       <c r="G10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>4</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>159</v>
       </c>
       <c r="I11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>5</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>172</v>
       </c>
       <c r="I12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F13" s="1" t="s">
-        <v>98</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C13" s="1"/>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F14" s="1" t="s">
-        <v>30</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="C14" s="1"/>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>164</v>
       </c>
       <c r="I14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>3</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
       </c>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
       <c r="I15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G17" t="s">
+      <c r="I16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="I17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E23">
-        <v>1111</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H23" t="s">
-        <v>105</v>
-      </c>
-      <c r="I23" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>109</v>
-      </c>
-      <c r="F24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24">
-        <v>1111</v>
-      </c>
-      <c r="H24" t="s">
-        <v>110</v>
-      </c>
-      <c r="I24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E25">
-        <v>111</v>
-      </c>
-      <c r="F25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25">
-        <v>1111</v>
-      </c>
-      <c r="H25" t="s">
-        <v>111</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26">
-        <v>500</v>
-      </c>
-      <c r="F26" t="s">
-        <v>108</v>
-      </c>
-      <c r="G26">
-        <v>1111</v>
-      </c>
-      <c r="H26" t="s">
-        <v>112</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G27">
-        <v>1111</v>
-      </c>
-      <c r="H27" t="s">
-        <v>113</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G28">
-        <v>1111</v>
-      </c>
-      <c r="H28" t="s">
-        <v>114</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>18</v>
-      </c>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C23" s="9"/>
+      <c r="D23" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1412,6 +1407,164 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EF03A8-C01B-4EC5-9622-342E1F504EDA}">
+  <dimension ref="C3:O47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="O4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="O5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D047279D-6843-4792-A616-C081EA17B349}">
   <dimension ref="A3:H15"/>
   <sheetViews>
@@ -1478,7 +1631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F71A6B84-5801-4404-B126-D1C859154014}">
   <dimension ref="B3:O72"/>
   <sheetViews>
@@ -1506,74 +1659,74 @@
   <sheetData>
     <row r="3" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C3" s="12" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>99</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C5" s="12" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="D6" s="12" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="D7" s="12" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="46.8" x14ac:dyDescent="0.3">
       <c r="D8" s="12" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -1582,46 +1735,46 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="12" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="12" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="J15" s="17"/>
       <c r="K15" s="15" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="N15" s="14" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="O15" s="13" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
@@ -1629,27 +1782,27 @@
         <v>1</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D16" s="12">
         <v>1212</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="14" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="12" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="L16" s="12">
         <v>2</v>
@@ -1658,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
@@ -1666,27 +1819,27 @@
         <v>2</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D17" s="12">
         <v>123132</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="12">
         <v>1</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="I17" s="12">
         <v>2</v>
       </c>
       <c r="J17" s="17"/>
       <c r="K17" s="12" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="L17" s="12">
         <v>3</v>
@@ -1695,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
@@ -1703,27 +1856,27 @@
         <v>3</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D18" s="12">
         <v>123123</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="12">
         <v>2</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="I18" s="12">
         <v>1</v>
       </c>
       <c r="J18" s="17"/>
       <c r="K18" s="12" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="L18" s="12">
         <v>1</v>
@@ -1732,7 +1885,7 @@
         <v>3</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
@@ -1740,27 +1893,27 @@
         <v>4</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="D19" s="12">
         <v>12313</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="12">
         <v>3</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="I19" s="12">
         <v>3</v>
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="12" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="L19" s="12">
         <v>2</v>
@@ -1769,7 +1922,7 @@
         <v>4</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
@@ -1777,27 +1930,27 @@
         <v>5</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D20" s="12">
         <v>323</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="12">
         <v>4</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="I20" s="12">
         <v>4</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="L20" s="12">
         <v>1</v>
@@ -1806,7 +1959,7 @@
         <v>5</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
@@ -1815,11 +1968,11 @@
         <v>5</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="L21" s="12">
         <v>2</v>
@@ -1828,7 +1981,7 @@
         <v>6</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
@@ -1837,11 +1990,11 @@
         <v>6</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="L22" s="12">
         <v>3</v>
@@ -1850,7 +2003,7 @@
         <v>7</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
@@ -1859,11 +2012,11 @@
         <v>7</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="J23" s="17"/>
       <c r="K23" s="12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="L23" s="12">
         <v>4</v>
@@ -1873,7 +2026,7 @@
       <c r="F24" s="17"/>
       <c r="J24" s="17"/>
       <c r="K24" s="12" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="L24" s="12">
         <v>4</v>
@@ -1883,7 +2036,7 @@
       <c r="F25" s="17"/>
       <c r="J25" s="17"/>
       <c r="K25" s="12" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="L25" s="12">
         <v>2</v>
@@ -1893,7 +2046,7 @@
       <c r="F26" s="17"/>
       <c r="J26" s="17"/>
       <c r="K26" s="12" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="L26" s="12">
         <v>4</v>
@@ -1913,56 +2066,56 @@
     </row>
     <row r="30" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B30" s="12" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="L30" s="13"/>
     </row>
     <row r="31" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C33" s="12" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.3">
@@ -1970,19 +2123,19 @@
         <v>1</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E38" s="19">
         <v>1212</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G38" s="18">
         <v>1</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="I38" s="18">
         <v>2</v>
@@ -1993,19 +2146,19 @@
         <v>2</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E39" s="20">
         <v>123132</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G39" s="21">
         <v>1</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="I39" s="21">
         <v>2</v>
@@ -2016,19 +2169,19 @@
         <v>3</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E40" s="19">
         <v>123123</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G40" s="18">
         <v>1</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="I40" s="18">
         <v>2</v>
@@ -2039,19 +2192,19 @@
         <v>4</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E41" s="19">
         <v>12313</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G41" s="18">
         <v>1</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="I41" s="18">
         <v>2</v>
@@ -2062,19 +2215,19 @@
         <v>5</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E42" s="19">
         <v>323</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G42" s="18">
         <v>1</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="I42" s="18">
         <v>2</v>
@@ -2085,19 +2238,19 @@
         <v>1</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E43" s="20">
         <v>1212</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G43" s="21">
         <v>2</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="I43" s="21">
         <v>1</v>
@@ -2108,19 +2261,19 @@
         <v>2</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E44" s="19">
         <v>123132</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G44" s="18">
         <v>2</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="I44" s="18">
         <v>1</v>
@@ -2131,19 +2284,19 @@
         <v>3</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E45" s="19">
         <v>123123</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G45" s="18">
         <v>2</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="I45" s="18">
         <v>1</v>
@@ -2154,19 +2307,19 @@
         <v>4</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E46" s="19">
         <v>12313</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G46" s="18">
         <v>2</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="I46" s="18">
         <v>1</v>
@@ -2177,19 +2330,19 @@
         <v>5</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E47" s="19">
         <v>323</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G47" s="18">
         <v>2</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="I47" s="18">
         <v>1</v>
@@ -2200,42 +2353,42 @@
         <v>1</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E48" s="19">
         <v>1212</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G48" s="18">
         <v>3</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="I48" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C49" s="19">
         <v>2</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E49" s="19">
         <v>123132</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G49" s="18">
         <v>3</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="I49" s="18">
         <v>3</v>
@@ -2246,19 +2399,19 @@
         <v>3</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E50" s="20">
         <v>123123</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G50" s="21">
         <v>3</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="I50" s="21">
         <v>3</v>
@@ -2269,19 +2422,19 @@
         <v>4</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E51" s="19">
         <v>12313</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G51" s="18">
         <v>3</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="I51" s="18">
         <v>3</v>
@@ -2292,19 +2445,19 @@
         <v>5</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E52" s="19">
         <v>323</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G52" s="18">
         <v>3</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="I52" s="18">
         <v>3</v>
@@ -2315,42 +2468,42 @@
         <v>1</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E53" s="19">
         <v>1212</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G53" s="18">
         <v>4</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="I53" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C54" s="19">
         <v>2</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E54" s="19">
         <v>123132</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G54" s="18">
         <v>4</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="I54" s="18">
         <v>4</v>
@@ -2361,19 +2514,19 @@
         <v>3</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E55" s="19">
         <v>123123</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G55" s="18">
         <v>4</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="I55" s="18">
         <v>4</v>
@@ -2384,19 +2537,19 @@
         <v>4</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E56" s="20">
         <v>12313</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G56" s="21">
         <v>4</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="I56" s="21">
         <v>4</v>
@@ -2407,19 +2560,19 @@
         <v>5</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E57" s="19">
         <v>323</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G57" s="18">
         <v>4</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="I57" s="18">
         <v>4</v>
@@ -2430,45 +2583,45 @@
         <v>1</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E58" s="19">
         <v>1212</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G58" s="18">
         <v>5</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C59" s="19">
         <v>2</v>
       </c>
       <c r="D59" s="19" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E59" s="19">
         <v>123132</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G59" s="18">
         <v>5</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="I59" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="3:9" x14ac:dyDescent="0.3">
@@ -2476,22 +2629,22 @@
         <v>3</v>
       </c>
       <c r="D60" s="19" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E60" s="19">
         <v>123123</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G60" s="18">
         <v>5</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="I60" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="3:9" x14ac:dyDescent="0.3">
@@ -2499,22 +2652,22 @@
         <v>4</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E61" s="19">
         <v>12313</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G61" s="18">
         <v>5</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="I61" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.3">
@@ -2522,22 +2675,22 @@
         <v>5</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E62" s="19">
         <v>323</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G62" s="18">
         <v>5</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="I62" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.3">
@@ -2545,45 +2698,45 @@
         <v>1</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E63" s="19">
         <v>1212</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G63" s="18">
         <v>6</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="I63" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="64" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C64" s="19">
         <v>2</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E64" s="19">
         <v>123132</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G64" s="18">
         <v>6</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="I64" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.3">
@@ -2591,22 +2744,22 @@
         <v>3</v>
       </c>
       <c r="D65" s="19" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E65" s="19">
         <v>123123</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G65" s="18">
         <v>6</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="I65" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.3">
@@ -2614,22 +2767,22 @@
         <v>4</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E66" s="19">
         <v>12313</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G66" s="18">
         <v>6</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.3">
@@ -2637,22 +2790,22 @@
         <v>5</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E67" s="19">
         <v>323</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G67" s="18">
         <v>6</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="I67" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="3:9" x14ac:dyDescent="0.3">
@@ -2660,45 +2813,45 @@
         <v>1</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E68" s="19">
         <v>1212</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="G68" s="18">
         <v>7</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="I68" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="69" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C69" s="19">
         <v>2</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E69" s="19">
         <v>123132</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="G69" s="18">
         <v>7</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="I69" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.3">
@@ -2706,22 +2859,22 @@
         <v>3</v>
       </c>
       <c r="D70" s="19" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E70" s="19">
         <v>123123</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G70" s="18">
         <v>7</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="I70" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.3">
@@ -2729,22 +2882,22 @@
         <v>4</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E71" s="19">
         <v>12313</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="G71" s="18">
         <v>7</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="I71" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.3">
@@ -2752,22 +2905,22 @@
         <v>5</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="E72" s="19">
         <v>323</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G72" s="18">
         <v>7</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="I72" s="18" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2776,22 +2929,34 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBCD982-A1F7-4F12-9554-A4111D34D39C}">
-  <dimension ref="A3:G8"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="37" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" customWidth="1"/>
+    <col min="6" max="6" width="57.5546875" customWidth="1"/>
+    <col min="7" max="7" width="43.77734375" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2810,8 +2975,11 @@
       <c r="F3" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>77</v>
       </c>
@@ -2821,8 +2989,11 @@
       <c r="F4" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>89</v>
       </c>
@@ -2830,10 +3001,13 @@
         <v>82</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D6" s="4" t="s">
         <v>88</v>
       </c>
@@ -2843,11 +3017,12 @@
       <c r="F6" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D7" s="4" t="s">
         <v>88</v>
       </c>
@@ -2855,18 +3030,98 @@
         <v>85</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G7" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>90</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>91</v>
+        <v>197</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" t="s">
+        <v>185</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" t="s">
+        <v>187</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2876,7 +3131,14 @@
     <hyperlink ref="F7" r:id="rId3" xr:uid="{D0EBD89A-D66D-4DE7-86DF-5DFE6CF72550}"/>
     <hyperlink ref="F8" r:id="rId4" xr:uid="{18C25863-A0B6-42AA-9649-2C7EF3D9B6E3}"/>
     <hyperlink ref="F5" r:id="rId5" xr:uid="{3B0BBC9D-C2D9-4372-8F28-57C51CE84779}"/>
+    <hyperlink ref="F12" r:id="rId6" xr:uid="{23D62CBE-F913-48E1-BB61-011CC1B0AF3A}"/>
+    <hyperlink ref="F13" r:id="rId7" xr:uid="{5D7C7235-0931-41A4-8D9C-A25FED980A75}"/>
+    <hyperlink ref="F14" r:id="rId8" xr:uid="{6E5D5C64-149F-469D-8FC2-C6D6F15B429A}"/>
+    <hyperlink ref="F15" r:id="rId9" xr:uid="{690443BB-935C-4306-975F-AD350037CCE8}"/>
+    <hyperlink ref="F16" r:id="rId10" xr:uid="{35BFFB03-C142-47BD-897D-7983C61F6FCE}"/>
+    <hyperlink ref="F17" r:id="rId11" xr:uid="{A6AD5FE8-090D-469D-B831-49F3D53948E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
9th August 2022 - Session
</commit_message>
<xml_diff>
--- a/Online Exam DB Plan.xlsx
+++ b/Online Exam DB Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ns_neutron\neutron_sql_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9863D66D-0DB8-492F-981E-8A86A740334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F0E902-213D-497E-9ED2-0266FD0DB17C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
   </bookViews>
@@ -314,9 +314,6 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>http://localhost:4000/users/updateuser</t>
-  </si>
-  <si>
     <t>Types of keys</t>
   </si>
   <si>
@@ -648,6 +645,9 @@
   </si>
   <si>
     <t>TYPE</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/users/updateuserpassword</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1127,7 @@
   <dimension ref="C3:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1180,10 +1180,10 @@
       </c>
       <c r="O3" s="22"/>
       <c r="P3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="R3" s="22"/>
     </row>
@@ -1198,13 +1198,13 @@
         <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="3:18" x14ac:dyDescent="0.3">
@@ -1215,13 +1215,13 @@
         <v>28</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" t="s">
         <v>156</v>
-      </c>
-      <c r="G5" t="s">
-        <v>170</v>
-      </c>
-      <c r="I5" t="s">
-        <v>157</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>20</v>
@@ -1238,7 +1238,7 @@
         <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K6" t="s">
         <v>41</v>
@@ -1255,7 +1255,7 @@
         <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.3">
@@ -1269,7 +1269,7 @@
         <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="3:18" x14ac:dyDescent="0.3">
@@ -1283,7 +1283,7 @@
         <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.3">
@@ -1297,7 +1297,7 @@
         <v>47</v>
       </c>
       <c r="G10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.3">
@@ -1311,10 +1311,10 @@
         <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="3:18" x14ac:dyDescent="0.3">
@@ -1325,10 +1325,10 @@
         <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.3">
@@ -1340,10 +1340,10 @@
         <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="3:18" x14ac:dyDescent="0.3">
@@ -1355,10 +1355,10 @@
         <v>51</v>
       </c>
       <c r="G14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="3:18" x14ac:dyDescent="0.3">
@@ -1369,10 +1369,10 @@
         <v>52</v>
       </c>
       <c r="G15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="3:18" x14ac:dyDescent="0.3">
@@ -1380,7 +1380,7 @@
         <v>72</v>
       </c>
       <c r="I16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.3">
@@ -1388,7 +1388,7 @@
         <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.3">
@@ -1421,17 +1421,17 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.3">
       <c r="O4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.3">
       <c r="O5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.3">
@@ -1659,74 +1659,74 @@
   <sheetData>
     <row r="3" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C3" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>108</v>
-      </c>
       <c r="E3" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="H4" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="46.8" x14ac:dyDescent="0.3">
       <c r="C5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="12" t="s">
         <v>103</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="D6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>105</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="D7" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="46.8" x14ac:dyDescent="0.3">
       <c r="D8" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -1735,46 +1735,46 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J15" s="17"/>
       <c r="K15" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="O15" s="13" t="s">
         <v>116</v>
-      </c>
-      <c r="L15" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="N15" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="O15" s="13" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
@@ -1782,27 +1782,27 @@
         <v>1</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" s="12">
         <v>1212</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F16" s="17"/>
       <c r="G16" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>117</v>
-      </c>
       <c r="I16" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L16" s="12">
         <v>2</v>
@@ -1811,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
@@ -1819,27 +1819,27 @@
         <v>2</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17" s="12">
         <v>123132</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="12">
         <v>1</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I17" s="12">
         <v>2</v>
       </c>
       <c r="J17" s="17"/>
       <c r="K17" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L17" s="12">
         <v>3</v>
@@ -1848,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="O17" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
@@ -1856,27 +1856,27 @@
         <v>3</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D18" s="12">
         <v>123123</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="12">
         <v>2</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I18" s="12">
         <v>1</v>
       </c>
       <c r="J18" s="17"/>
       <c r="K18" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L18" s="12">
         <v>1</v>
@@ -1885,7 +1885,7 @@
         <v>3</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
@@ -1893,27 +1893,27 @@
         <v>4</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" s="12">
         <v>12313</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="12">
         <v>3</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I19" s="12">
         <v>3</v>
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L19" s="12">
         <v>2</v>
@@ -1922,7 +1922,7 @@
         <v>4</v>
       </c>
       <c r="O19" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
@@ -1930,27 +1930,27 @@
         <v>5</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D20" s="12">
         <v>323</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="12">
         <v>4</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I20" s="12">
         <v>4</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L20" s="12">
         <v>1</v>
@@ -1959,7 +1959,7 @@
         <v>5</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
@@ -1968,11 +1968,11 @@
         <v>5</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L21" s="12">
         <v>2</v>
@@ -1981,7 +1981,7 @@
         <v>6</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
@@ -1990,11 +1990,11 @@
         <v>6</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L22" s="12">
         <v>3</v>
@@ -2003,7 +2003,7 @@
         <v>7</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
@@ -2012,11 +2012,11 @@
         <v>7</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J23" s="17"/>
       <c r="K23" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L23" s="12">
         <v>4</v>
@@ -2026,7 +2026,7 @@
       <c r="F24" s="17"/>
       <c r="J24" s="17"/>
       <c r="K24" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L24" s="12">
         <v>4</v>
@@ -2036,7 +2036,7 @@
       <c r="F25" s="17"/>
       <c r="J25" s="17"/>
       <c r="K25" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L25" s="12">
         <v>2</v>
@@ -2046,7 +2046,7 @@
       <c r="F26" s="17"/>
       <c r="J26" s="17"/>
       <c r="K26" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L26" s="12">
         <v>4</v>
@@ -2066,56 +2066,56 @@
     </row>
     <row r="30" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B30" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F30" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="H30" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="I30" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="I30" s="13" t="s">
+      <c r="J30" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="J30" s="13" t="s">
+      <c r="K30" s="13" t="s">
         <v>144</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>145</v>
       </c>
       <c r="L30" s="13"/>
     </row>
     <row r="31" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="2:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="3:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="C33" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.3">
@@ -2123,19 +2123,19 @@
         <v>1</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E38" s="19">
         <v>1212</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G38" s="18">
         <v>1</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I38" s="18">
         <v>2</v>
@@ -2146,19 +2146,19 @@
         <v>2</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E39" s="20">
         <v>123132</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G39" s="21">
         <v>1</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I39" s="21">
         <v>2</v>
@@ -2169,19 +2169,19 @@
         <v>3</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E40" s="19">
         <v>123123</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G40" s="18">
         <v>1</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I40" s="18">
         <v>2</v>
@@ -2192,19 +2192,19 @@
         <v>4</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E41" s="19">
         <v>12313</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G41" s="18">
         <v>1</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I41" s="18">
         <v>2</v>
@@ -2215,19 +2215,19 @@
         <v>5</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E42" s="19">
         <v>323</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G42" s="18">
         <v>1</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I42" s="18">
         <v>2</v>
@@ -2238,19 +2238,19 @@
         <v>1</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E43" s="20">
         <v>1212</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G43" s="21">
         <v>2</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I43" s="21">
         <v>1</v>
@@ -2261,19 +2261,19 @@
         <v>2</v>
       </c>
       <c r="D44" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E44" s="19">
         <v>123132</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G44" s="18">
         <v>2</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I44" s="18">
         <v>1</v>
@@ -2284,19 +2284,19 @@
         <v>3</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E45" s="19">
         <v>123123</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G45" s="18">
         <v>2</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I45" s="18">
         <v>1</v>
@@ -2307,19 +2307,19 @@
         <v>4</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E46" s="19">
         <v>12313</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G46" s="18">
         <v>2</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I46" s="18">
         <v>1</v>
@@ -2330,19 +2330,19 @@
         <v>5</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E47" s="19">
         <v>323</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G47" s="18">
         <v>2</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I47" s="18">
         <v>1</v>
@@ -2353,19 +2353,19 @@
         <v>1</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E48" s="19">
         <v>1212</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G48" s="18">
         <v>3</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I48" s="18">
         <v>3</v>
@@ -2376,19 +2376,19 @@
         <v>2</v>
       </c>
       <c r="D49" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E49" s="19">
         <v>123132</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G49" s="18">
         <v>3</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I49" s="18">
         <v>3</v>
@@ -2399,19 +2399,19 @@
         <v>3</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E50" s="20">
         <v>123123</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G50" s="21">
         <v>3</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I50" s="21">
         <v>3</v>
@@ -2422,19 +2422,19 @@
         <v>4</v>
       </c>
       <c r="D51" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E51" s="19">
         <v>12313</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G51" s="18">
         <v>3</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I51" s="18">
         <v>3</v>
@@ -2445,19 +2445,19 @@
         <v>5</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E52" s="19">
         <v>323</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G52" s="18">
         <v>3</v>
       </c>
       <c r="H52" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I52" s="18">
         <v>3</v>
@@ -2468,19 +2468,19 @@
         <v>1</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E53" s="19">
         <v>1212</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G53" s="18">
         <v>4</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I53" s="18">
         <v>4</v>
@@ -2491,19 +2491,19 @@
         <v>2</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E54" s="19">
         <v>123132</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G54" s="18">
         <v>4</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I54" s="18">
         <v>4</v>
@@ -2514,19 +2514,19 @@
         <v>3</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E55" s="19">
         <v>123123</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G55" s="18">
         <v>4</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I55" s="18">
         <v>4</v>
@@ -2537,19 +2537,19 @@
         <v>4</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E56" s="20">
         <v>12313</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G56" s="21">
         <v>4</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I56" s="21">
         <v>4</v>
@@ -2560,19 +2560,19 @@
         <v>5</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E57" s="19">
         <v>323</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G57" s="18">
         <v>4</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I57" s="18">
         <v>4</v>
@@ -2583,22 +2583,22 @@
         <v>1</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E58" s="19">
         <v>1212</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G58" s="18">
         <v>5</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="3:9" x14ac:dyDescent="0.3">
@@ -2606,22 +2606,22 @@
         <v>2</v>
       </c>
       <c r="D59" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E59" s="19">
         <v>123132</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G59" s="18">
         <v>5</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I59" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="3:9" x14ac:dyDescent="0.3">
@@ -2629,22 +2629,22 @@
         <v>3</v>
       </c>
       <c r="D60" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E60" s="19">
         <v>123123</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G60" s="18">
         <v>5</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I60" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="3:9" x14ac:dyDescent="0.3">
@@ -2652,22 +2652,22 @@
         <v>4</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E61" s="19">
         <v>12313</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G61" s="18">
         <v>5</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I61" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.3">
@@ -2675,22 +2675,22 @@
         <v>5</v>
       </c>
       <c r="D62" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E62" s="19">
         <v>323</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G62" s="18">
         <v>5</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I62" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.3">
@@ -2698,22 +2698,22 @@
         <v>1</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E63" s="19">
         <v>1212</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G63" s="18">
         <v>6</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I63" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.3">
@@ -2721,22 +2721,22 @@
         <v>2</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E64" s="19">
         <v>123132</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G64" s="18">
         <v>6</v>
       </c>
       <c r="H64" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I64" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.3">
@@ -2744,22 +2744,22 @@
         <v>3</v>
       </c>
       <c r="D65" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E65" s="19">
         <v>123123</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G65" s="18">
         <v>6</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I65" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.3">
@@ -2767,22 +2767,22 @@
         <v>4</v>
       </c>
       <c r="D66" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E66" s="19">
         <v>12313</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G66" s="18">
         <v>6</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.3">
@@ -2790,22 +2790,22 @@
         <v>5</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E67" s="19">
         <v>323</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G67" s="18">
         <v>6</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I67" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="3:9" x14ac:dyDescent="0.3">
@@ -2813,22 +2813,22 @@
         <v>1</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E68" s="19">
         <v>1212</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G68" s="18">
         <v>7</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I68" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="3:9" x14ac:dyDescent="0.3">
@@ -2836,22 +2836,22 @@
         <v>2</v>
       </c>
       <c r="D69" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E69" s="19">
         <v>123132</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G69" s="18">
         <v>7</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I69" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="3:9" x14ac:dyDescent="0.3">
@@ -2859,22 +2859,22 @@
         <v>3</v>
       </c>
       <c r="D70" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E70" s="19">
         <v>123123</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G70" s="18">
         <v>7</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I70" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.3">
@@ -2882,22 +2882,22 @@
         <v>4</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E71" s="19">
         <v>12313</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G71" s="18">
         <v>7</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I71" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.3">
@@ -2905,22 +2905,22 @@
         <v>5</v>
       </c>
       <c r="D72" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E72" s="19">
         <v>323</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G72" s="18">
         <v>7</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I72" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2934,7 +2934,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2947,64 +2947,64 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>198</v>
+      <c r="G5" s="5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -3030,7 +3030,7 @@
         <v>85</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="4" t="s">
@@ -3042,28 +3042,28 @@
         <v>90</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>191</v>
+      <c r="G12" s="5" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -3071,13 +3071,13 @@
         <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -3085,43 +3085,43 @@
         <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>189</v>
-      </c>
-      <c r="E15" t="s">
-        <v>185</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>